<commit_message>
added diffence in excel and json
</commit_message>
<xml_diff>
--- a/tst.xlsx
+++ b/tst.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -710,6 +710,206 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>111</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>111555</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2222</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>22333332</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>22</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>224</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>33</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>customername</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Customer's Name</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>pii</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>